<commit_message>
updated blur parameter and added more data to spreadsheet for blurred cases
</commit_message>
<xml_diff>
--- a/manual.xlsx
+++ b/manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/finch/merrygoround/school/24fl/shapes/final/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\CSE554\napari-measure-drosophila-sperm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC9B729-B32D-CC4F-AAD6-140CEA5B7817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80B2C87-0084-4A4A-98D3-BFB335882462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="500" windowWidth="10740" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>53387.1B.2_7&amp;8</t>
   </si>
@@ -187,6 +187,18 @@
   </si>
   <si>
     <t>driver -&gt; skeleton -&gt; remove small objs(minsize=15)</t>
+  </si>
+  <si>
+    <t>with blur</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>minsize=100</t>
+  </si>
+  <si>
+    <t>minsize=90</t>
   </si>
 </sst>
 </file>
@@ -247,7 +259,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +281,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,8 +344,8 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,9 +365,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -387,9 +405,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,26 +440,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,26 +475,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -667,29 +651,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="9"/>
-    <col min="2" max="2" width="16.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="9"/>
+    <col min="2" max="2" width="16.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" style="10" customWidth="1"/>
     <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.1640625" style="1"/>
-    <col min="13" max="13" width="20" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="8.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.109375" style="1"/>
+    <col min="13" max="13" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
@@ -726,8 +710,20 @@
       <c r="M1" s="14" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -741,7 +737,7 @@
         <v>1061</v>
       </c>
       <c r="E2" s="10">
-        <f>D2/C2</f>
+        <f t="shared" ref="E2:E13" si="0">D2/C2</f>
         <v>0.74627705518089305</v>
       </c>
       <c r="F2" s="10">
@@ -753,7 +749,7 @@
         <v>839</v>
       </c>
       <c r="K2" s="17">
-        <f>J2/C2</f>
+        <f t="shared" ref="K2:K13" si="1">J2/C2</f>
         <v>0.59012860442673831</v>
       </c>
       <c r="L2" s="20">
@@ -763,8 +759,16 @@
       <c r="M2" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R2" s="10">
+        <f t="shared" ref="R2:R22" si="2">Q2/C2</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="20">
+        <f t="shared" ref="S2:S22" si="3">ABS((Q2-C2)/C2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -775,11 +779,11 @@
         <v>1591</v>
       </c>
       <c r="E3" s="10">
-        <f>D3/C3</f>
+        <f t="shared" si="0"/>
         <v>0.92434436039553336</v>
       </c>
       <c r="F3" s="10">
-        <f t="shared" ref="F3:F23" si="0">ABS((D3-C3)/C3)</f>
+        <f t="shared" ref="F3:F23" si="4">ABS((D3-C3)/C3)</f>
         <v>7.5655639604466612E-2</v>
       </c>
       <c r="G3" s="2"/>
@@ -787,15 +791,23 @@
         <v>1367</v>
       </c>
       <c r="K3" s="10">
-        <f>J3/C3</f>
+        <f t="shared" si="1"/>
         <v>0.79420411103751987</v>
       </c>
       <c r="L3" s="20">
-        <f t="shared" ref="L3:L23" si="1">ABS((J3-C3)/C3)</f>
+        <f t="shared" ref="L3:L23" si="5">ABS((J3-C3)/C3)</f>
         <v>0.20579588896248011</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R3" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S3" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
@@ -806,11 +818,11 @@
         <v>1728</v>
       </c>
       <c r="E4" s="10">
-        <f>D4/C4</f>
+        <f t="shared" si="0"/>
         <v>0.96100585279258954</v>
       </c>
       <c r="F4" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.8994147207410415E-2</v>
       </c>
       <c r="G4" s="3"/>
@@ -818,15 +830,23 @@
         <v>1712</v>
       </c>
       <c r="K4" s="10">
-        <f>J4/C4</f>
+        <f t="shared" si="1"/>
         <v>0.95210765045191748</v>
       </c>
       <c r="L4" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>4.7892349548082538E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R4" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -837,11 +857,11 @@
         <v>1833</v>
       </c>
       <c r="E5" s="10">
-        <f>D5/C5</f>
+        <f t="shared" si="0"/>
         <v>1.0069165775383444</v>
       </c>
       <c r="F5" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6.9165775383443467E-3</v>
       </c>
       <c r="G5" s="3"/>
@@ -849,15 +869,29 @@
         <v>1880</v>
       </c>
       <c r="K5" s="10">
-        <f>J5/C5</f>
+        <f t="shared" si="1"/>
         <v>1.0327349513213788</v>
       </c>
       <c r="L5" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.2734951321378818E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1">
+        <v>1875</v>
+      </c>
+      <c r="R5" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0299883158125454</v>
+      </c>
+      <c r="S5" s="20">
+        <f t="shared" si="3"/>
+        <v>2.9988315812545362E-2</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -868,11 +902,11 @@
         <v>1453</v>
       </c>
       <c r="E6" s="10">
-        <f>D6/C6</f>
+        <f t="shared" si="0"/>
         <v>0.79507262903651199</v>
       </c>
       <c r="F6" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.20492737096348798</v>
       </c>
       <c r="G6" s="2"/>
@@ -880,15 +914,23 @@
         <v>1462</v>
       </c>
       <c r="K6" s="10">
-        <f>J6/C6</f>
+        <f t="shared" si="1"/>
         <v>0.79999737346963562</v>
       </c>
       <c r="L6" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.20000262653036438</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R6" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -899,11 +941,11 @@
         <v>1083</v>
       </c>
       <c r="E7" s="17">
-        <f>D7/C7</f>
+        <f t="shared" si="0"/>
         <v>0.5897430451978416</v>
       </c>
       <c r="F7" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.41025695480215835</v>
       </c>
       <c r="G7" s="2"/>
@@ -911,15 +953,26 @@
         <v>1068</v>
       </c>
       <c r="K7" s="17">
-        <f>J7/C7</f>
+        <f t="shared" si="1"/>
         <v>0.58157485897626493</v>
       </c>
       <c r="L7" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.41842514102373513</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q7" s="22">
+        <v>1044</v>
+      </c>
+      <c r="R7" s="10">
+        <f t="shared" si="2"/>
+        <v>0.56850576102174211</v>
+      </c>
+      <c r="S7" s="20">
+        <f t="shared" si="3"/>
+        <v>0.43149423897825795</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -930,11 +983,11 @@
         <v>800</v>
       </c>
       <c r="E8" s="17">
-        <f>D8/C8</f>
+        <f t="shared" si="0"/>
         <v>0.43474196977239082</v>
       </c>
       <c r="F8" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.56525803022760912</v>
       </c>
       <c r="G8" s="2">
@@ -951,18 +1004,26 @@
         <v>790</v>
       </c>
       <c r="K8" s="17">
-        <f>J8/C8</f>
+        <f t="shared" si="1"/>
         <v>0.42930769515023592</v>
       </c>
       <c r="L8" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.57069230484976408</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R8" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
@@ -973,11 +1034,11 @@
         <v>1259</v>
       </c>
       <c r="E9" s="17">
-        <f>D9/C9</f>
+        <f t="shared" si="0"/>
         <v>0.68164591229020033</v>
       </c>
       <c r="F9" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.31835408770979967</v>
       </c>
       <c r="G9" s="2"/>
@@ -988,18 +1049,26 @@
         <v>1254</v>
       </c>
       <c r="K9" s="17">
-        <f>J9/C9</f>
+        <f t="shared" si="1"/>
         <v>0.67893881970763403</v>
       </c>
       <c r="L9" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.32106118029236602</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R9" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S9" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1010,11 +1079,11 @@
         <v>1381</v>
       </c>
       <c r="E10" s="10">
-        <f>D10/C10</f>
+        <f t="shared" si="0"/>
         <v>0.74673553287772187</v>
       </c>
       <c r="F10" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.25326446712227807</v>
       </c>
       <c r="G10" s="2">
@@ -1031,15 +1100,23 @@
         <v>1381</v>
       </c>
       <c r="K10" s="10">
-        <f>J10/C10</f>
+        <f t="shared" si="1"/>
         <v>0.74673553287772187</v>
       </c>
       <c r="L10" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.25326446712227807</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R10" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S10" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1050,11 +1127,11 @@
         <v>1301</v>
       </c>
       <c r="E11" s="19">
-        <f>D11/C11</f>
+        <f t="shared" si="0"/>
         <v>0.70324476377246214</v>
       </c>
       <c r="F11" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.2967552362275378</v>
       </c>
       <c r="G11" s="2">
@@ -1071,18 +1148,26 @@
         <v>1285</v>
       </c>
       <c r="K11" s="19">
-        <f>J11/C11</f>
+        <f t="shared" si="1"/>
         <v>0.69459609642399223</v>
       </c>
       <c r="L11" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.30540390357600777</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R11" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S11" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1093,11 +1178,11 @@
         <v>1950</v>
       </c>
       <c r="E12" s="10">
-        <f>D12/C12</f>
+        <f t="shared" si="0"/>
         <v>1.042323686939417</v>
       </c>
       <c r="F12" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4.2323686939416974E-2</v>
       </c>
       <c r="G12" s="2"/>
@@ -1108,15 +1193,23 @@
         <v>1753</v>
       </c>
       <c r="K12" s="10">
-        <f>J12/C12</f>
+        <f t="shared" si="1"/>
         <v>0.93702226831015278</v>
       </c>
       <c r="L12" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6.2977731689847202E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R12" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S12" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
@@ -1127,11 +1220,11 @@
         <v>1897</v>
       </c>
       <c r="E13" s="10">
-        <f>D13/C13</f>
+        <f t="shared" si="0"/>
         <v>1.0123780156537017</v>
       </c>
       <c r="F13" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.2378015653701589E-2</v>
       </c>
       <c r="G13" s="2"/>
@@ -1142,20 +1235,30 @@
         <v>1978</v>
       </c>
       <c r="K13" s="10">
-        <f>J13/C13</f>
+        <f t="shared" si="1"/>
         <v>1.0556055429430795</v>
       </c>
       <c r="L13" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5.5605542943079463E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R13" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="J14" s="13"/>
       <c r="K14" s="10"/>
       <c r="L14" s="20"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R14" s="10"/>
+      <c r="S14" s="20"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
@@ -1173,7 +1276,7 @@
         <v>0.92563950029744202</v>
       </c>
       <c r="F15" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7.4360499702557994E-2</v>
       </c>
       <c r="J15" s="13">
@@ -1184,11 +1287,19 @@
         <v>0.99464604402141588</v>
       </c>
       <c r="L15" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5.353955978584176E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R15" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
@@ -1203,7 +1314,7 @@
         <v>1.0348360655737705</v>
       </c>
       <c r="F16" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.4836065573770489E-2</v>
       </c>
       <c r="J16" s="13">
@@ -1214,14 +1325,25 @@
         <v>1.1818647540983607</v>
       </c>
       <c r="L16" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.18186475409836064</v>
       </c>
       <c r="M16" s="18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q16" s="1">
+        <v>2111</v>
+      </c>
+      <c r="R16" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0814549180327868</v>
+      </c>
+      <c r="S16" s="20">
+        <f t="shared" si="3"/>
+        <v>8.1454918032786885E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
@@ -1236,7 +1358,7 @@
         <v>1.4239075841285787</v>
       </c>
       <c r="F17" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.4239075841285786</v>
       </c>
       <c r="G17" s="1">
@@ -1257,14 +1379,22 @@
         <v>1.2847815168257157</v>
       </c>
       <c r="L17" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.28478151682571573</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R17" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S17" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
@@ -1279,7 +1409,7 @@
         <v>0.97339449541284406</v>
       </c>
       <c r="F18" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2.6605504587155965E-2</v>
       </c>
       <c r="J18" s="13">
@@ -1290,14 +1420,22 @@
         <v>0.76330275229357802</v>
       </c>
       <c r="L18" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.23669724770642203</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R18" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
@@ -1312,7 +1450,7 @@
         <v>1.6242555495397943</v>
       </c>
       <c r="F19" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.62425554953979423</v>
       </c>
       <c r="G19" s="1">
@@ -1333,19 +1471,29 @@
         <v>1.0184082295614509</v>
       </c>
       <c r="L19" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.8408229561451002E-2</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R19" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S19" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="J20" s="13"/>
       <c r="K20" s="10"/>
       <c r="L20" s="20"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R20" s="10"/>
+      <c r="S20" s="20"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>16</v>
       </c>
@@ -1363,7 +1511,7 @@
         <v>0.84623270117888261</v>
       </c>
       <c r="F21" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.15376729882111737</v>
       </c>
       <c r="J21" s="13">
@@ -1374,14 +1522,22 @@
         <v>0.97796002050230646</v>
       </c>
       <c r="L21" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.2039979497693492E-2</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R21" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S21" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
@@ -1392,11 +1548,11 @@
         <v>1615</v>
       </c>
       <c r="E22" s="10">
-        <f t="shared" ref="E22:E23" si="2">D22/C22</f>
+        <f t="shared" ref="E22:E23" si="6">D22/C22</f>
         <v>0.90374930050363733</v>
       </c>
       <c r="F22" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.6250699496362613E-2</v>
       </c>
       <c r="J22" s="13">
@@ -1407,11 +1563,19 @@
         <v>1.0290990486849469</v>
       </c>
       <c r="L22" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.9099048684946838E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R22" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S22" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>24</v>
       </c>
@@ -1422,11 +1586,11 @@
         <v>1756</v>
       </c>
       <c r="E23" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.98320268756998885</v>
       </c>
       <c r="F23" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.6797312430011199E-2</v>
       </c>
       <c r="J23" s="13">
@@ -1437,42 +1601,53 @@
         <v>1.0699888017917134</v>
       </c>
       <c r="L23" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6.9988801791713323E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L24" s="21"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q23" s="1">
+        <v>1643</v>
+      </c>
+      <c r="R23" s="10">
+        <f>Q23/C23</f>
+        <v>0.91993281075027999</v>
+      </c>
+      <c r="S23" s="20">
+        <f>ABS((Q23-C23)/C23)</f>
+        <v>8.0067189249720047E-2</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F25" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="L25" s="21" t="s">
+      <c r="L25" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F26" s="10">
         <f>AVERAGE(F3:F23)</f>
         <v>0.19346656464608206</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="21">
         <f>AVERAGE(L3:L23)</f>
         <v>0.1748468222107511</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E27" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K28" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K29" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
manual measure adds point on top of image and added another tesing column to spreadsheet
</commit_message>
<xml_diff>
--- a/manual.xlsx
+++ b/manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/finch/merrygoround/school/24fl/shapes/final/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\CSE554\napari-measure-drosophila-sperm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC9B729-B32D-CC4F-AAD6-140CEA5B7817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FAFE44-4F29-4BD6-8276-912DB487C74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="500" windowWidth="10740" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-6660" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>53387.1B.2_7&amp;8</t>
   </si>
@@ -187,6 +187,36 @@
   </si>
   <si>
     <t>driver -&gt; skeleton -&gt; remove small objs(minsize=15)</t>
+  </si>
+  <si>
+    <t>minsize=13</t>
+  </si>
+  <si>
+    <t>minsize=114</t>
+  </si>
+  <si>
+    <t>minsize=10</t>
+  </si>
+  <si>
+    <t>minsize=130</t>
+  </si>
+  <si>
+    <t>minsize=40</t>
+  </si>
+  <si>
+    <t>minsize=20</t>
+  </si>
+  <si>
+    <t>minsize=10, top is 1565</t>
+  </si>
+  <si>
+    <t>minsize=5</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>new thresh</t>
   </si>
 </sst>
 </file>
@@ -286,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -326,7 +356,6 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -347,9 +376,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -387,9 +416,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,26 +451,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,26 +486,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -667,29 +662,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="9"/>
-    <col min="2" max="2" width="16.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="9"/>
+    <col min="2" max="2" width="16.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" style="10" customWidth="1"/>
     <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.1640625" style="1"/>
+    <col min="10" max="12" width="9.109375" style="1"/>
     <col min="13" max="13" width="20" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="1"/>
+    <col min="14" max="16" width="9.109375" style="1"/>
+    <col min="17" max="17" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
@@ -726,8 +723,20 @@
       <c r="M1" s="14" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -741,7 +750,7 @@
         <v>1061</v>
       </c>
       <c r="E2" s="10">
-        <f>D2/C2</f>
+        <f t="shared" ref="E2:E13" si="0">D2/C2</f>
         <v>0.74627705518089305</v>
       </c>
       <c r="F2" s="10">
@@ -753,7 +762,7 @@
         <v>839</v>
       </c>
       <c r="K2" s="17">
-        <f>J2/C2</f>
+        <f t="shared" ref="K2:K13" si="1">J2/C2</f>
         <v>0.59012860442673831</v>
       </c>
       <c r="L2" s="20">
@@ -763,8 +772,22 @@
       <c r="M2" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q2" s="1">
+        <v>1144</v>
+      </c>
+      <c r="R2" s="10">
+        <f t="shared" ref="R2:R22" si="2">Q2/C2</f>
+        <v>0.8046568813637528</v>
+      </c>
+      <c r="S2" s="20">
+        <f t="shared" ref="S2:S22" si="3">ABS((Q2-C2)/C2)</f>
+        <v>0.19534311863624723</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -775,11 +798,11 @@
         <v>1591</v>
       </c>
       <c r="E3" s="10">
-        <f>D3/C3</f>
+        <f t="shared" si="0"/>
         <v>0.92434436039553336</v>
       </c>
       <c r="F3" s="10">
-        <f t="shared" ref="F3:F23" si="0">ABS((D3-C3)/C3)</f>
+        <f t="shared" ref="F3:F23" si="4">ABS((D3-C3)/C3)</f>
         <v>7.5655639604466612E-2</v>
       </c>
       <c r="G3" s="2"/>
@@ -787,15 +810,29 @@
         <v>1367</v>
       </c>
       <c r="K3" s="10">
-        <f>J3/C3</f>
+        <f t="shared" si="1"/>
         <v>0.79420411103751987</v>
       </c>
       <c r="L3" s="20">
-        <f t="shared" ref="L3:L23" si="1">ABS((J3-C3)/C3)</f>
+        <f t="shared" ref="L3:L23" si="5">ABS((J3-C3)/C3)</f>
         <v>0.20579588896248011</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q3" s="1">
+        <v>1074</v>
+      </c>
+      <c r="R3" s="10">
+        <f t="shared" si="2"/>
+        <v>0.62397601701118977</v>
+      </c>
+      <c r="S3" s="20">
+        <f t="shared" si="3"/>
+        <v>0.37602398298881029</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
@@ -806,11 +843,11 @@
         <v>1728</v>
       </c>
       <c r="E4" s="10">
-        <f>D4/C4</f>
+        <f t="shared" si="0"/>
         <v>0.96100585279258954</v>
       </c>
       <c r="F4" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.8994147207410415E-2</v>
       </c>
       <c r="G4" s="3"/>
@@ -818,15 +855,29 @@
         <v>1712</v>
       </c>
       <c r="K4" s="10">
-        <f>J4/C4</f>
+        <f t="shared" si="1"/>
         <v>0.95210765045191748</v>
       </c>
       <c r="L4" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>4.7892349548082538E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1">
+        <v>1907</v>
+      </c>
+      <c r="R4" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0605544914788589</v>
+      </c>
+      <c r="S4" s="20">
+        <f t="shared" si="3"/>
+        <v>6.0554491478858989E-2</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -837,11 +888,11 @@
         <v>1833</v>
       </c>
       <c r="E5" s="10">
-        <f>D5/C5</f>
+        <f t="shared" si="0"/>
         <v>1.0069165775383444</v>
       </c>
       <c r="F5" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6.9165775383443467E-3</v>
       </c>
       <c r="G5" s="3"/>
@@ -849,15 +900,29 @@
         <v>1880</v>
       </c>
       <c r="K5" s="10">
-        <f>J5/C5</f>
+        <f t="shared" si="1"/>
         <v>1.0327349513213788</v>
       </c>
       <c r="L5" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.2734951321378818E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1">
+        <v>1975</v>
+      </c>
+      <c r="R5" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0849210259892144</v>
+      </c>
+      <c r="S5" s="20">
+        <f t="shared" si="3"/>
+        <v>8.4921025989214444E-2</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -868,11 +933,11 @@
         <v>1453</v>
       </c>
       <c r="E6" s="10">
-        <f>D6/C6</f>
+        <f t="shared" si="0"/>
         <v>0.79507262903651199</v>
       </c>
       <c r="F6" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.20492737096348798</v>
       </c>
       <c r="G6" s="2"/>
@@ -880,15 +945,29 @@
         <v>1462</v>
       </c>
       <c r="K6" s="10">
-        <f>J6/C6</f>
+        <f t="shared" si="1"/>
         <v>0.79999737346963562</v>
       </c>
       <c r="L6" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.20000262653036438</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q6" s="1">
+        <v>1352</v>
+      </c>
+      <c r="R6" s="10">
+        <f t="shared" si="2"/>
+        <v>0.73980605262034704</v>
+      </c>
+      <c r="S6" s="20">
+        <f t="shared" si="3"/>
+        <v>0.26019394737965296</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -899,11 +978,11 @@
         <v>1083</v>
       </c>
       <c r="E7" s="17">
-        <f>D7/C7</f>
+        <f t="shared" si="0"/>
         <v>0.5897430451978416</v>
       </c>
       <c r="F7" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.41025695480215835</v>
       </c>
       <c r="G7" s="2"/>
@@ -911,15 +990,29 @@
         <v>1068</v>
       </c>
       <c r="K7" s="17">
-        <f>J7/C7</f>
+        <f t="shared" si="1"/>
         <v>0.58157485897626493</v>
       </c>
       <c r="L7" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.41842514102373513</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q7" s="1">
+        <v>1507</v>
+      </c>
+      <c r="R7" s="10">
+        <f t="shared" si="2"/>
+        <v>0.82063044239441119</v>
+      </c>
+      <c r="S7" s="20">
+        <f t="shared" si="3"/>
+        <v>0.17936955760558879</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -930,11 +1023,11 @@
         <v>800</v>
       </c>
       <c r="E8" s="17">
-        <f>D8/C8</f>
+        <f t="shared" si="0"/>
         <v>0.43474196977239082</v>
       </c>
       <c r="F8" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.56525803022760912</v>
       </c>
       <c r="G8" s="2">
@@ -951,18 +1044,32 @@
         <v>790</v>
       </c>
       <c r="K8" s="17">
-        <f>J8/C8</f>
+        <f t="shared" si="1"/>
         <v>0.42930769515023592</v>
       </c>
       <c r="L8" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.57069230484976408</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <v>705</v>
+      </c>
+      <c r="R8" s="10">
+        <f t="shared" si="2"/>
+        <v>0.38311636086191941</v>
+      </c>
+      <c r="S8" s="20">
+        <f t="shared" si="3"/>
+        <v>0.61688363913808053</v>
+      </c>
+      <c r="T8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
@@ -973,11 +1080,11 @@
         <v>1259</v>
       </c>
       <c r="E9" s="17">
-        <f>D9/C9</f>
+        <f t="shared" si="0"/>
         <v>0.68164591229020033</v>
       </c>
       <c r="F9" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.31835408770979967</v>
       </c>
       <c r="G9" s="2"/>
@@ -988,18 +1095,32 @@
         <v>1254</v>
       </c>
       <c r="K9" s="17">
-        <f>J9/C9</f>
+        <f t="shared" si="1"/>
         <v>0.67893881970763403</v>
       </c>
       <c r="L9" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.32106118029236602</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q9">
+        <v>1615</v>
+      </c>
+      <c r="R9" s="10">
+        <f t="shared" si="2"/>
+        <v>0.87439090416892262</v>
+      </c>
+      <c r="S9" s="20">
+        <f t="shared" si="3"/>
+        <v>0.12560909583107743</v>
+      </c>
+      <c r="T9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1010,11 +1131,11 @@
         <v>1381</v>
       </c>
       <c r="E10" s="10">
-        <f>D10/C10</f>
+        <f t="shared" si="0"/>
         <v>0.74673553287772187</v>
       </c>
       <c r="F10" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.25326446712227807</v>
       </c>
       <c r="G10" s="2">
@@ -1031,15 +1152,29 @@
         <v>1381</v>
       </c>
       <c r="K10" s="10">
-        <f>J10/C10</f>
+        <f t="shared" si="1"/>
         <v>0.74673553287772187</v>
       </c>
       <c r="L10" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.25326446712227807</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q10">
+        <v>1655</v>
+      </c>
+      <c r="R10" s="10">
+        <f t="shared" si="2"/>
+        <v>0.89489305352109327</v>
+      </c>
+      <c r="S10" s="20">
+        <f t="shared" si="3"/>
+        <v>0.10510694647890677</v>
+      </c>
+      <c r="T10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1050,11 +1185,11 @@
         <v>1301</v>
       </c>
       <c r="E11" s="19">
-        <f>D11/C11</f>
+        <f t="shared" si="0"/>
         <v>0.70324476377246214</v>
       </c>
       <c r="F11" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.2967552362275378</v>
       </c>
       <c r="G11" s="2">
@@ -1071,18 +1206,29 @@
         <v>1285</v>
       </c>
       <c r="K11" s="19">
-        <f>J11/C11</f>
+        <f t="shared" si="1"/>
         <v>0.69459609642399223</v>
       </c>
       <c r="L11" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.30540390357600777</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q11" s="1">
+        <v>1426</v>
+      </c>
+      <c r="R11" s="10">
+        <f t="shared" si="2"/>
+        <v>0.77081247743238357</v>
+      </c>
+      <c r="S11" s="20">
+        <f t="shared" si="3"/>
+        <v>0.2291875225676164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1093,11 +1239,11 @@
         <v>1950</v>
       </c>
       <c r="E12" s="10">
-        <f>D12/C12</f>
+        <f t="shared" si="0"/>
         <v>1.042323686939417</v>
       </c>
       <c r="F12" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4.2323686939416974E-2</v>
       </c>
       <c r="G12" s="2"/>
@@ -1108,15 +1254,29 @@
         <v>1753</v>
       </c>
       <c r="K12" s="10">
-        <f>J12/C12</f>
+        <f t="shared" si="1"/>
         <v>0.93702226831015278</v>
       </c>
       <c r="L12" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6.2977731689847202E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q12" s="1">
+        <v>1942</v>
+      </c>
+      <c r="R12" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0380474871981271</v>
+      </c>
+      <c r="S12" s="20">
+        <f t="shared" si="3"/>
+        <v>3.8047487198127061E-2</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
@@ -1127,11 +1287,11 @@
         <v>1897</v>
       </c>
       <c r="E13" s="10">
-        <f>D13/C13</f>
+        <f t="shared" si="0"/>
         <v>1.0123780156537017</v>
       </c>
       <c r="F13" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.2378015653701589E-2</v>
       </c>
       <c r="G13" s="2"/>
@@ -1142,20 +1302,36 @@
         <v>1978</v>
       </c>
       <c r="K13" s="10">
-        <f>J13/C13</f>
+        <f t="shared" si="1"/>
         <v>1.0556055429430795</v>
       </c>
       <c r="L13" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5.5605542943079463E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q13">
+        <v>1968</v>
+      </c>
+      <c r="R13" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0502688111789587</v>
+      </c>
+      <c r="S13" s="20">
+        <f t="shared" si="3"/>
+        <v>5.026881117895874E-2</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="J14" s="13"/>
       <c r="K14" s="10"/>
       <c r="L14" s="20"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R14" s="10"/>
+      <c r="S14" s="20"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
@@ -1173,7 +1349,7 @@
         <v>0.92563950029744202</v>
       </c>
       <c r="F15" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7.4360499702557994E-2</v>
       </c>
       <c r="J15" s="13">
@@ -1184,11 +1360,22 @@
         <v>0.99464604402141588</v>
       </c>
       <c r="L15" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5.353955978584176E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q15" s="1">
+        <v>1780</v>
+      </c>
+      <c r="R15" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0588935157644259</v>
+      </c>
+      <c r="S15" s="20">
+        <f t="shared" si="3"/>
+        <v>5.889351576442594E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
@@ -1203,7 +1390,7 @@
         <v>1.0348360655737705</v>
       </c>
       <c r="F16" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.4836065573770489E-2</v>
       </c>
       <c r="J16" s="13">
@@ -1214,14 +1401,25 @@
         <v>1.1818647540983607</v>
       </c>
       <c r="L16" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.18186475409836064</v>
       </c>
       <c r="M16" s="18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q16" s="1">
+        <v>2293</v>
+      </c>
+      <c r="R16" s="10">
+        <f t="shared" si="2"/>
+        <v>1.1746926229508197</v>
+      </c>
+      <c r="S16" s="20">
+        <f t="shared" si="3"/>
+        <v>0.17469262295081966</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
@@ -1236,7 +1434,7 @@
         <v>1.4239075841285787</v>
       </c>
       <c r="F17" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.4239075841285786</v>
       </c>
       <c r="G17" s="1">
@@ -1257,14 +1455,25 @@
         <v>1.2847815168257157</v>
       </c>
       <c r="L17" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.28478151682571573</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q17" s="1">
+        <v>2444</v>
+      </c>
+      <c r="R17" s="10">
+        <f t="shared" si="2"/>
+        <v>1.2275238573581115</v>
+      </c>
+      <c r="S17" s="20">
+        <f t="shared" si="3"/>
+        <v>0.22752385735811151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
@@ -1279,7 +1488,7 @@
         <v>0.97339449541284406</v>
       </c>
       <c r="F18" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2.6605504587155965E-2</v>
       </c>
       <c r="J18" s="13">
@@ -1290,14 +1499,28 @@
         <v>0.76330275229357802</v>
       </c>
       <c r="L18" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.23669724770642203</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q18">
+        <v>1189</v>
+      </c>
+      <c r="R18" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0908256880733944</v>
+      </c>
+      <c r="S18" s="20">
+        <f t="shared" si="3"/>
+        <v>9.08256880733945E-2</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
@@ -1312,7 +1535,7 @@
         <v>1.6242555495397943</v>
       </c>
       <c r="F19" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.62425554953979423</v>
       </c>
       <c r="G19" s="1">
@@ -1333,19 +1556,35 @@
         <v>1.0184082295614509</v>
       </c>
       <c r="L19" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.8408229561451002E-2</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q19">
+        <v>1977</v>
+      </c>
+      <c r="R19" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0703844071467243</v>
+      </c>
+      <c r="S19" s="20">
+        <f t="shared" si="3"/>
+        <v>7.038440714672442E-2</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="J20" s="13"/>
       <c r="K20" s="10"/>
       <c r="L20" s="20"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R20" s="10"/>
+      <c r="S20" s="20"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>16</v>
       </c>
@@ -1363,7 +1602,7 @@
         <v>0.84623270117888261</v>
       </c>
       <c r="F21" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.15376729882111737</v>
       </c>
       <c r="J21" s="13">
@@ -1374,14 +1613,25 @@
         <v>0.97796002050230646</v>
       </c>
       <c r="L21" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.2039979497693492E-2</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q21" s="1">
+        <v>1918</v>
+      </c>
+      <c r="R21" s="10">
+        <f t="shared" si="2"/>
+        <v>0.98308559712967714</v>
+      </c>
+      <c r="S21" s="20">
+        <f t="shared" si="3"/>
+        <v>1.6914402870322913E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
@@ -1392,11 +1642,11 @@
         <v>1615</v>
       </c>
       <c r="E22" s="10">
-        <f t="shared" ref="E22:E23" si="2">D22/C22</f>
+        <f t="shared" ref="E22:E23" si="6">D22/C22</f>
         <v>0.90374930050363733</v>
       </c>
       <c r="F22" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.6250699496362613E-2</v>
       </c>
       <c r="J22" s="13">
@@ -1407,11 +1657,22 @@
         <v>1.0290990486849469</v>
       </c>
       <c r="L22" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.9099048684946838E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q22" s="1">
+        <v>1754</v>
+      </c>
+      <c r="R22" s="10">
+        <f t="shared" si="2"/>
+        <v>0.98153329602686068</v>
+      </c>
+      <c r="S22" s="20">
+        <f t="shared" si="3"/>
+        <v>1.8466703973139341E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>24</v>
       </c>
@@ -1422,11 +1683,11 @@
         <v>1756</v>
       </c>
       <c r="E23" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.98320268756998885</v>
       </c>
       <c r="F23" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.6797312430011199E-2</v>
       </c>
       <c r="J23" s="13">
@@ -1437,42 +1698,50 @@
         <v>1.0699888017917134</v>
       </c>
       <c r="L23" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6.9988801791713323E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L24" s="21"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q23" s="13">
+        <v>1754</v>
+      </c>
+      <c r="R23" s="10">
+        <f>Q23/C23</f>
+        <v>0.98208286674132139</v>
+      </c>
+      <c r="S23" s="20">
+        <f>ABS((Q23-C23)/C23)</f>
+        <v>1.7917133258678612E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F25" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="L25" s="21" t="s">
+      <c r="L25" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F26" s="10">
         <f>AVERAGE(F3:F23)</f>
         <v>0.19346656464608206</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="21">
         <f>AVERAGE(L3:L23)</f>
         <v>0.1748468222107511</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E27" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K28" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K29" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>